<commit_message>
Dev Updates from Anjali 11/15 - 11p IST
</commit_message>
<xml_diff>
--- a/xls-templates/proposal-template.xlsx
+++ b/xls-templates/proposal-template.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="12840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="50">
   <si>
     <t>&lt;/jx:forEach&gt;</t>
   </si>
@@ -141,9 +136,6 @@
     <t>${disclaimer}</t>
   </si>
   <si>
-    <t>&lt;jx:forEach items="${exporter.getDisclaimers('Chicago - Flight 1', 'Chicago', 'Bulletin')}" var="disclaimer"&gt;</t>
-  </si>
-  <si>
     <t>Important notes</t>
   </si>
   <si>
@@ -163,51 +155,41 @@
   </si>
   <si>
     <t>&lt;jx:if test="${exporter.excludeNetworkDetails == false}"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:if test="${exporter.getDisclaimers(group.item.flight.name, group.item.flight.division, group.item.flight.mediaCategory, group.item.additionalCostFieldSelected, group.item.additionalCost, group.item.additionalCostType)}"&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;/jx:if&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${exporter.getDisclaimers()}" var="disclaimer"&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -219,26 +201,26 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -266,16 +248,16 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -295,284 +277,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="119">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -589,19 +339,25 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>608463</xdr:colOff>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>295062</xdr:rowOff>
+      <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -610,17 +366,34 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="85725" y="47625"/>
-          <a:ext cx="2999238" cy="247437"/>
+          <a:ext cx="2924175" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln w="9525">
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
+        <a:ln>
+          <a:noFill/>
         </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -629,7 +402,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -703,6 +476,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -737,6 +511,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -912,31 +687,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D94"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95:XFD95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="15.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="15.7109375" style="1"/>
+    <col min="1" max="16384" width="15.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29.45" customHeight="1"/>
-    <row r="2" spans="1:4" ht="14.45" customHeight="1">
+    <row r="1" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="5" spans="1:4" ht="14.1" customHeight="1" thickTop="1" thickBot="1">
+    <row r="4" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:4" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -950,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.45" customHeight="1" thickTop="1">
+    <row r="6" spans="1:4" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>36</v>
       </c>
@@ -964,23 +739,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.45" customHeight="1">
+    <row r="7" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.45" customHeight="1">
+    <row r="8" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.45" customHeight="1">
+    <row r="9" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.45" customHeight="1" thickBot="1"/>
-    <row r="11" spans="1:4" ht="14.45" customHeight="1" thickTop="1" thickBot="1">
+    <row r="10" spans="1:4" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:4" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
@@ -994,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickTop="1">
+    <row r="12" spans="1:4" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
@@ -1008,27 +783,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1">
+    <row r="17" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>3</v>
       </c>
@@ -1042,17 +817,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickTop="1">
+    <row r="19" spans="1:4" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1">
+    <row r="20" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>3</v>
       </c>
@@ -1066,17 +841,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickTop="1">
+    <row r="22" spans="1:4" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1">
+    <row r="23" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>3</v>
       </c>
@@ -1090,17 +865,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickTop="1">
+    <row r="25" spans="1:4" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1">
+    <row r="26" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>3</v>
       </c>
@@ -1114,27 +889,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickTop="1">
+    <row r="28" spans="1:4" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>6</v>
       </c>
@@ -1148,17 +923,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
@@ -1172,17 +947,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>6</v>
       </c>
@@ -1196,17 +971,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>6</v>
       </c>
@@ -1220,33 +995,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1">
+    <row r="47" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>17</v>
       </c>
@@ -1257,17 +1032,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickTop="1">
+    <row r="49" spans="1:3" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1">
+    <row r="50" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
@@ -1278,17 +1053,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" thickTop="1">
+    <row r="52" spans="1:3" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1">
+    <row r="53" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>23</v>
       </c>
@@ -1299,22 +1074,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" thickTop="1">
+    <row r="55" spans="1:3" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A57" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+    <row r="58" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>22</v>
       </c>
@@ -1325,32 +1100,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" thickTop="1">
+    <row r="59" spans="1:3" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>16</v>
       </c>
@@ -1361,17 +1136,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>19</v>
       </c>
@@ -1382,17 +1157,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>24</v>
       </c>
@@ -1403,22 +1178,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" thickBot="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>22</v>
       </c>
@@ -1429,13 +1204,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" s="9" customFormat="1" ht="15.75" thickTop="1">
+    <row r="75" spans="1:3" s="9" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B75" s="8"/>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>21</v>
       </c>
@@ -1446,12 +1221,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.75" thickBot="1">
+    <row r="77" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>26</v>
       </c>
@@ -1462,12 +1237,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.75" thickTop="1">
+    <row r="79" spans="1:3" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A79" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
         <v>27</v>
       </c>
@@ -1478,76 +1253,336 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:256" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:256" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:256" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:256" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
+    <row r="86" spans="1:256" x14ac:dyDescent="0.15">
+      <c r="A86" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="87" spans="1:256" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:256" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:256" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="1" t="s">
+    <row r="90" spans="1:256" x14ac:dyDescent="0.15">
+      <c r="A90" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:256" x14ac:dyDescent="0.15">
+      <c r="A91" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="92" spans="1:256" x14ac:dyDescent="0.15">
+      <c r="A92" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="11"/>
+      <c r="I92" s="11"/>
+      <c r="J92" s="11"/>
+      <c r="K92" s="11"/>
+      <c r="L92" s="11"/>
+      <c r="M92" s="11"/>
+      <c r="N92" s="11"/>
+      <c r="O92" s="11"/>
+      <c r="P92" s="11"/>
+      <c r="Q92" s="11"/>
+      <c r="R92" s="11"/>
+      <c r="S92" s="11"/>
+      <c r="T92" s="11"/>
+      <c r="U92" s="11"/>
+      <c r="V92" s="11"/>
+      <c r="W92" s="11"/>
+      <c r="X92" s="11"/>
+      <c r="Y92" s="11"/>
+      <c r="Z92" s="11"/>
+      <c r="AA92" s="11"/>
+      <c r="AB92" s="11"/>
+      <c r="AC92" s="11"/>
+      <c r="AD92" s="11"/>
+      <c r="AE92" s="11"/>
+      <c r="AF92" s="11"/>
+      <c r="AG92" s="11"/>
+      <c r="AH92" s="11"/>
+      <c r="AI92" s="11"/>
+      <c r="AJ92" s="11"/>
+      <c r="AK92" s="11"/>
+      <c r="AL92" s="11"/>
+      <c r="AM92" s="11"/>
+      <c r="AN92" s="11"/>
+      <c r="AO92" s="11"/>
+      <c r="AP92" s="11"/>
+      <c r="AQ92" s="11"/>
+      <c r="AR92" s="11"/>
+      <c r="AS92" s="11"/>
+      <c r="AT92" s="11"/>
+      <c r="AU92" s="11"/>
+      <c r="AV92" s="11"/>
+      <c r="AW92" s="11"/>
+      <c r="AX92" s="11"/>
+      <c r="AY92" s="11"/>
+      <c r="AZ92" s="11"/>
+      <c r="BA92" s="11"/>
+      <c r="BB92" s="11"/>
+      <c r="BC92" s="11"/>
+      <c r="BD92" s="11"/>
+      <c r="BE92" s="11"/>
+      <c r="BF92" s="11"/>
+      <c r="BG92" s="11"/>
+      <c r="BH92" s="11"/>
+      <c r="BI92" s="11"/>
+      <c r="BJ92" s="11"/>
+      <c r="BK92" s="11"/>
+      <c r="BL92" s="11"/>
+      <c r="BM92" s="11"/>
+      <c r="BN92" s="11"/>
+      <c r="BO92" s="11"/>
+      <c r="BP92" s="11"/>
+      <c r="BQ92" s="11"/>
+      <c r="BR92" s="11"/>
+      <c r="BS92" s="11"/>
+      <c r="BT92" s="11"/>
+      <c r="BU92" s="11"/>
+      <c r="BV92" s="11"/>
+      <c r="BW92" s="11"/>
+      <c r="BX92" s="11"/>
+      <c r="BY92" s="11"/>
+      <c r="BZ92" s="11"/>
+      <c r="CA92" s="11"/>
+      <c r="CB92" s="11"/>
+      <c r="CC92" s="11"/>
+      <c r="CD92" s="11"/>
+      <c r="CE92" s="11"/>
+      <c r="CF92" s="11"/>
+      <c r="CG92" s="11"/>
+      <c r="CH92" s="11"/>
+      <c r="CI92" s="11"/>
+      <c r="CJ92" s="11"/>
+      <c r="CK92" s="11"/>
+      <c r="CL92" s="11"/>
+      <c r="CM92" s="11"/>
+      <c r="CN92" s="11"/>
+      <c r="CO92" s="11"/>
+      <c r="CP92" s="11"/>
+      <c r="CQ92" s="11"/>
+      <c r="CR92" s="11"/>
+      <c r="CS92" s="11"/>
+      <c r="CT92" s="11"/>
+      <c r="CU92" s="11"/>
+      <c r="CV92" s="11"/>
+      <c r="CW92" s="11"/>
+      <c r="CX92" s="11"/>
+      <c r="CY92" s="11"/>
+      <c r="CZ92" s="11"/>
+      <c r="DA92" s="11"/>
+      <c r="DB92" s="11"/>
+      <c r="DC92" s="11"/>
+      <c r="DD92" s="11"/>
+      <c r="DE92" s="11"/>
+      <c r="DF92" s="11"/>
+      <c r="DG92" s="11"/>
+      <c r="DH92" s="11"/>
+      <c r="DI92" s="11"/>
+      <c r="DJ92" s="11"/>
+      <c r="DK92" s="11"/>
+      <c r="DL92" s="11"/>
+      <c r="DM92" s="11"/>
+      <c r="DN92" s="11"/>
+      <c r="DO92" s="11"/>
+      <c r="DP92" s="11"/>
+      <c r="DQ92" s="11"/>
+      <c r="DR92" s="11"/>
+      <c r="DS92" s="11"/>
+      <c r="DT92" s="11"/>
+      <c r="DU92" s="11"/>
+      <c r="DV92" s="11"/>
+      <c r="DW92" s="11"/>
+      <c r="DX92" s="11"/>
+      <c r="DY92" s="11"/>
+      <c r="DZ92" s="11"/>
+      <c r="EA92" s="11"/>
+      <c r="EB92" s="11"/>
+      <c r="EC92" s="11"/>
+      <c r="ED92" s="11"/>
+      <c r="EE92" s="11"/>
+      <c r="EF92" s="11"/>
+      <c r="EG92" s="11"/>
+      <c r="EH92" s="11"/>
+      <c r="EI92" s="11"/>
+      <c r="EJ92" s="11"/>
+      <c r="EK92" s="11"/>
+      <c r="EL92" s="11"/>
+      <c r="EM92" s="11"/>
+      <c r="EN92" s="11"/>
+      <c r="EO92" s="11"/>
+      <c r="EP92" s="11"/>
+      <c r="EQ92" s="11"/>
+      <c r="ER92" s="11"/>
+      <c r="ES92" s="11"/>
+      <c r="ET92" s="11"/>
+      <c r="EU92" s="11"/>
+      <c r="EV92" s="11"/>
+      <c r="EW92" s="11"/>
+      <c r="EX92" s="11"/>
+      <c r="EY92" s="11"/>
+      <c r="EZ92" s="11"/>
+      <c r="FA92" s="11"/>
+      <c r="FB92" s="11"/>
+      <c r="FC92" s="11"/>
+      <c r="FD92" s="11"/>
+      <c r="FE92" s="11"/>
+      <c r="FF92" s="11"/>
+      <c r="FG92" s="11"/>
+      <c r="FH92" s="11"/>
+      <c r="FI92" s="11"/>
+      <c r="FJ92" s="11"/>
+      <c r="FK92" s="11"/>
+      <c r="FL92" s="11"/>
+      <c r="FM92" s="11"/>
+      <c r="FN92" s="11"/>
+      <c r="FO92" s="11"/>
+      <c r="FP92" s="11"/>
+      <c r="FQ92" s="11"/>
+      <c r="FR92" s="11"/>
+      <c r="FS92" s="11"/>
+      <c r="FT92" s="11"/>
+      <c r="FU92" s="11"/>
+      <c r="FV92" s="11"/>
+      <c r="FW92" s="11"/>
+      <c r="FX92" s="11"/>
+      <c r="FY92" s="11"/>
+      <c r="FZ92" s="11"/>
+      <c r="GA92" s="11"/>
+      <c r="GB92" s="11"/>
+      <c r="GC92" s="11"/>
+      <c r="GD92" s="11"/>
+      <c r="GE92" s="11"/>
+      <c r="GF92" s="11"/>
+      <c r="GG92" s="11"/>
+      <c r="GH92" s="11"/>
+      <c r="GI92" s="11"/>
+      <c r="GJ92" s="11"/>
+      <c r="GK92" s="11"/>
+      <c r="GL92" s="11"/>
+      <c r="GM92" s="11"/>
+      <c r="GN92" s="11"/>
+      <c r="GO92" s="11"/>
+      <c r="GP92" s="11"/>
+      <c r="GQ92" s="11"/>
+      <c r="GR92" s="11"/>
+      <c r="GS92" s="11"/>
+      <c r="GT92" s="11"/>
+      <c r="GU92" s="11"/>
+      <c r="GV92" s="11"/>
+      <c r="GW92" s="11"/>
+      <c r="GX92" s="11"/>
+      <c r="GY92" s="11"/>
+      <c r="GZ92" s="11"/>
+      <c r="HA92" s="11"/>
+      <c r="HB92" s="11"/>
+      <c r="HC92" s="11"/>
+      <c r="HD92" s="11"/>
+      <c r="HE92" s="11"/>
+      <c r="HF92" s="11"/>
+      <c r="HG92" s="11"/>
+      <c r="HH92" s="11"/>
+      <c r="HI92" s="11"/>
+      <c r="HJ92" s="11"/>
+      <c r="HK92" s="11"/>
+      <c r="HL92" s="11"/>
+      <c r="HM92" s="11"/>
+      <c r="HN92" s="11"/>
+      <c r="HO92" s="11"/>
+      <c r="HP92" s="11"/>
+      <c r="HQ92" s="11"/>
+      <c r="HR92" s="11"/>
+      <c r="HS92" s="11"/>
+      <c r="HT92" s="11"/>
+      <c r="HU92" s="11"/>
+      <c r="HV92" s="11"/>
+      <c r="HW92" s="11"/>
+      <c r="HX92" s="11"/>
+      <c r="HY92" s="11"/>
+      <c r="HZ92" s="11"/>
+      <c r="IA92" s="11"/>
+      <c r="IB92" s="11"/>
+      <c r="IC92" s="11"/>
+      <c r="ID92" s="11"/>
+      <c r="IE92" s="11"/>
+      <c r="IF92" s="11"/>
+      <c r="IG92" s="11"/>
+      <c r="IH92" s="11"/>
+      <c r="II92" s="11"/>
+      <c r="IJ92" s="11"/>
+      <c r="IK92" s="11"/>
+      <c r="IL92" s="11"/>
+      <c r="IM92" s="11"/>
+      <c r="IN92" s="11"/>
+      <c r="IO92" s="11"/>
+      <c r="IP92" s="11"/>
+      <c r="IQ92" s="11"/>
+      <c r="IR92" s="11"/>
+      <c r="IS92" s="11"/>
+      <c r="IT92" s="11"/>
+      <c r="IU92" s="11"/>
+      <c r="IV92" s="11"/>
+    </row>
+    <row r="93" spans="1:256" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:256" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:256" x14ac:dyDescent="0.15">
+      <c r="A95" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>